<commit_message>
Atualização do backlog e mudança na seção da equipe
</commit_message>
<xml_diff>
--- a/SITE OFICIAL/Documentação/Grupo 8 - ProductBacklog.xlsx
+++ b/SITE OFICIAL/Documentação/Grupo 8 - ProductBacklog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabes\Downloads\SIS 2°Semestre\PI - Fernando\SPRINT 1\Chech-In---Grupo8\Gabriela\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabes\Downloads\SIS 2°Semestre\PI - Fernando\SPRINT 1\Chech-In---Grupo8\SITE OFICIAL\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{436AD6FE-9158-4749-AF7B-C4F338C0DDC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49DCB2A0-607A-4724-B081-F2362EB457CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="121">
   <si>
     <t>Cód. do Requisito</t>
   </si>
@@ -58,9 +58,56 @@
     <t>US001</t>
   </si>
   <si>
-    <t>Em andamento</t>
-  </si>
-  <si>
+    <t>Planejada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O sistema deverá apresentar os dados em função do monitoramento dos totens. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Essencial </t>
+  </si>
+  <si>
+    <t>Ao usuário acessar a tela de monitoramento dos totens de autendimento ele terá acesso as dashboards em tempo real.</t>
+  </si>
+  <si>
+    <t>US003</t>
+  </si>
+  <si>
+    <t>O sistema deverá apresentar alertas e notificações sobre alterações advindas das dashboards.</t>
+  </si>
+  <si>
+    <t>Ao ser feito o monitoramento das dashboards, caso haja alguma alteração deverá ser enviado um alerta na tela para o usuário.</t>
+  </si>
+  <si>
+    <t>PROT001</t>
+  </si>
+  <si>
+    <t>Feito</t>
+  </si>
+  <si>
+    <t>O site deverá apresentar uma página de menus para a localização de mais informações sobre nossa empresa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Importante </t>
+  </si>
+  <si>
+    <t>Ao ser acessada pelo usuário, que irá se localizar pelo menu de páginas para obter mais infomações.</t>
+  </si>
+  <si>
+    <t>O site deverá apresentar uma seção de footer para que o usuário possa entrar em contato com nossa equipe.</t>
+  </si>
+  <si>
+    <t>Ao acessar as páginas do site o usuário terá de forma pratica o acesso ao footer para entrar em contato  com a equipe e tirar dúvidas.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t>O site deverá apresentar uma seção introdutória</t>
+    </r>
     <r>
       <rPr>
         <b/>
@@ -68,7 +115,7 @@
         <color rgb="FF000000"/>
         <rFont val="Barlow"/>
       </rPr>
-      <t xml:space="preserve">Tela de dashboard; </t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -76,19 +123,21 @@
         <color rgb="FF000000"/>
         <rFont val="Barlow"/>
       </rPr>
-      <t xml:space="preserve">é um requisito importante para a apresentação dos dados em função do monitoramento dos totens trazendo praticidade e reduzindo o tempo de resolução de problemas e bugs no sistema operacional </t>
+      <t>que apresenta inicialmente nossos serviços de forma rápida e objetiva.</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Importante </t>
-  </si>
-  <si>
-    <t>US003</t>
-  </si>
-  <si>
-    <t>Planejada</t>
-  </si>
-  <si>
+    <t>Ao acessar o site o usuário terá acesso a uma seção com informações sobre o projeto.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t>O site deverá apresentar uma seção com tópicos gerais</t>
+    </r>
     <r>
       <rPr>
         <b/>
@@ -96,7 +145,7 @@
         <color rgb="FF000000"/>
         <rFont val="Barlow"/>
       </rPr>
-      <t xml:space="preserve">Alertas/Notificações; </t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -104,16 +153,36 @@
         <color rgb="FF000000"/>
         <rFont val="Barlow"/>
       </rPr>
-      <t xml:space="preserve">é um requisito importante para caso seja necessária a interferência, devido alguma alteração repentina de alto ou médio grau nos componentes monitorados. </t>
+      <t>para que o usuário tenha uma visão geral sobre o que nossa equipe acredita para ter desenvolvido o projeto.</t>
     </r>
   </si>
   <si>
-    <t>PROT001</t>
-  </si>
-  <si>
-    <t>Feito</t>
-  </si>
-  <si>
+    <t>Ao acessar o site o usuário terá acesso a uma seção com tópicos nos quais a equipe acredita.</t>
+  </si>
+  <si>
+    <t>PROT002</t>
+  </si>
+  <si>
+    <t>O site deverá apresentar uma seção explicativa sobre nosso projeto, mostrando detalhes e a motivação pelo qual o projeto foi criado.</t>
+  </si>
+  <si>
+    <t>Ao acessar o site o usuário terá acesso a uma seção com mais detalhes sobre o projeto na tela sobre nós.</t>
+  </si>
+  <si>
+    <t>O site deverá apresentar uma seção de valores para que o cliente possa ter mais detalhes e passar maior credibilidade.</t>
+  </si>
+  <si>
+    <t>Ao acessar o site o usuário terá acesso a uma seção com os valores dos quais movem nosso projeto e passar confiança aos nossos futuros clientes.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t>O site deverá apresentar uma seção com apresentação da equipe</t>
+    </r>
     <r>
       <rPr>
         <b/>
@@ -121,7 +190,7 @@
         <color rgb="FF000000"/>
         <rFont val="Barlow"/>
       </rPr>
-      <t xml:space="preserve">Footer; </t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -129,10 +198,21 @@
         <color rgb="FF000000"/>
         <rFont val="Barlow"/>
       </rPr>
-      <t>é uma seção importante para que o usuário ao navegar pelo site tenha maior praticidade de encontrar informações e ser direcionario para outras seções do site.</t>
+      <t>para que o cliente possa conhecer e ter confiança que a equipe está preparada.</t>
     </r>
   </si>
   <si>
+    <t xml:space="preserve">Ao ser acessada a página (sobre nós) nossos usuário teram acesso a uma seção com os intergantes que pertencem a equipe e mostrar credibilidade aos clientes e usuários.  </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t>O site deverá apresentar uma seção de feedback</t>
+    </r>
     <r>
       <rPr>
         <b/>
@@ -140,7 +220,7 @@
         <color rgb="FF000000"/>
         <rFont val="Barlow"/>
       </rPr>
-      <t xml:space="preserve">Seção introdutória; </t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -148,10 +228,36 @@
         <color rgb="FF000000"/>
         <rFont val="Barlow"/>
       </rPr>
-      <t>é uma seção que apresenta inicialmente sobre nossos serviços de forma rápida e objetiva.</t>
+      <t>para que os novos clientes e/ou usuários possam ter acesso ao feedback de empresas que já são nossos clientes;</t>
     </r>
   </si>
   <si>
+    <t>Ao ser acessada a página (sobre nós) nossos clientes encontrarão uma seção com feedbacks de clientes que já contrataram nosso serviços, essa seção serve para que possamos ter mais credibilidade.</t>
+  </si>
+  <si>
+    <t>PROT003</t>
+  </si>
+  <si>
+    <t>Em Andamento</t>
+  </si>
+  <si>
+    <t>O site deverá apresentar uma seção de serviços para que caso os clientes tenham interesse em nossos serviços, previamente possam nos conhecer e entrar em contato.</t>
+  </si>
+  <si>
+    <t>Ao acessar o site o usuário terá uma página de serviços, onde encontrará todos os serviços realizados pela nossa empresa e o porque nos contratar.</t>
+  </si>
+  <si>
+    <t>PROT004</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t>O site deverá apresentar uma seção de contato</t>
+    </r>
     <r>
       <rPr>
         <b/>
@@ -159,7 +265,7 @@
         <color rgb="FF000000"/>
         <rFont val="Barlow"/>
       </rPr>
-      <t xml:space="preserve">Seção com tópicos gerais; </t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -167,16 +273,21 @@
         <color rgb="FF000000"/>
         <rFont val="Barlow"/>
       </rPr>
-      <t>é um requisito importante para que o usuário que tenha acesso ao site, tenha uma visão geral sobre o que nossa equipe acredita para ter desenvolvido o projeto.</t>
+      <t xml:space="preserve">para que o cliente tenha acesso aos nossos serviços e possa entrar em contato; </t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Essencial </t>
-  </si>
-  <si>
-    <t>PROT002</t>
-  </si>
-  <si>
+    <t>Ao acessar o site o cliente terá uma página de contato, para que possa nos contactar online ou via telefones.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t>O site deverá apresentar uma seção de login</t>
+    </r>
     <r>
       <rPr>
         <b/>
@@ -184,7 +295,7 @@
         <color rgb="FF000000"/>
         <rFont val="Barlow"/>
       </rPr>
-      <t>Seção explicativa;</t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -192,10 +303,30 @@
         <color rgb="FF000000"/>
         <rFont val="Barlow"/>
       </rPr>
-      <t xml:space="preserve"> é um requisito que explica sobre nosso projeto, mostrando detalhes e motivação pelo qual o projeto foi criado.</t>
+      <t>para que o cliente tenha acesso ao nosso principal serviço, sendo ele as dashboards.</t>
     </r>
   </si>
   <si>
+    <t>Ao fechar o contrato com nossa empresa, o cliente já cadastrado previamente em nossos bancos de dados possuirá uma página de login, para que possa ter acesso as dashboards relacionadas a sua empresa.</t>
+  </si>
+  <si>
+    <t>O site deverá apresentar uma seção de beneficios do negócio que apresenta ao usuário como nossos serviços funcionam e no que a equipe acredita.</t>
+  </si>
+  <si>
+    <t>A página trará para os usuários informações referente ao que acreditamos e porque nossos serviços funcionam.</t>
+  </si>
+  <si>
+    <t>PROT005</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t>O site deverá apresentar uma seção para ADM,</t>
+    </r>
     <r>
       <rPr>
         <b/>
@@ -203,7 +334,7 @@
         <color rgb="FF000000"/>
         <rFont val="Barlow"/>
       </rPr>
-      <t>Seção de valores;</t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -211,10 +342,27 @@
         <color rgb="FF000000"/>
         <rFont val="Barlow"/>
       </rPr>
-      <t xml:space="preserve"> é um requisito importante para que o cliente possa ter mais detalhes e passar maior credibilidade;</t>
+      <t>pois é através desta seção que o usuário administrador pode fazer a criação de outros usuários analistas.</t>
     </r>
   </si>
   <si>
+    <t>Essa seção será usada pelo nosso cliente ja cadastrado em nosso banco de dados, para que ele possa cadastrar funcionários de sua empresa que necessitam acessas nossos serviços para controle interno.</t>
+  </si>
+  <si>
+    <t>O site deverá apresentar uma seção de dashboard para Analista para que o responsavel da empresa possa ter acesso aos dados para tomada de decisão;</t>
+  </si>
+  <si>
+    <t>O acesso a essa seção será exclusivo para os usuários que ja tiverem efetuado login, serve para que nossos clientes tenham acesso em tempo real ao monitoramento de suas máquinas.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t>O site deverá apresentar uma seção de suporte</t>
+    </r>
     <r>
       <rPr>
         <b/>
@@ -222,7 +370,7 @@
         <color rgb="FF000000"/>
         <rFont val="Barlow"/>
       </rPr>
-      <t>Seção com apresentação da equipe;</t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -230,10 +378,30 @@
         <color rgb="FF000000"/>
         <rFont val="Barlow"/>
       </rPr>
-      <t xml:space="preserve"> é um requisito importante para o cliente possa conhecer e ter confiança que a equipe está preparada.</t>
+      <t>para que o usuário possa ter acesso a resolução de falhas e problemas nas dashboards.</t>
     </r>
   </si>
   <si>
+    <t>Nessa seção o cliente poderá entrar em contato com nossos colaboradores 24/7 para que sejam feitos reparos ou resolução de problemas.</t>
+  </si>
+  <si>
+    <t>O site deverá apresentar uma seção de cadastro para que o ADM possa ser cadastrado.</t>
+  </si>
+  <si>
+    <t>Essa página será utilizada pelos nossos colaboradores para realizar o cadastro dos nosso clientes em nosso banco de dados para que ele possa realizar seu login.</t>
+  </si>
+  <si>
+    <t>EC001</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t>O projeto deverá ter pesquisas de campo</t>
+    </r>
     <r>
       <rPr>
         <b/>
@@ -241,7 +409,7 @@
         <color rgb="FF000000"/>
         <rFont val="Barlow"/>
       </rPr>
-      <t xml:space="preserve">Seção de feedback; </t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -249,16 +417,57 @@
         <color rgb="FF000000"/>
         <rFont val="Barlow"/>
       </rPr>
-      <t>é um requisito importante para que os novos clientes e/ou usuários possam ter acesso ao feedback de empresas já são nossos clientes;</t>
+      <t>para que a equipe possa identificar problemas, falhas e bugs nos sistemas operacionais dos totens de autoatendimento.</t>
     </r>
   </si>
   <si>
-    <t>PROT003</t>
-  </si>
-  <si>
-    <t>Em Andamento</t>
-  </si>
-  <si>
+    <t>Desejável</t>
+  </si>
+  <si>
+    <t>Essa ação consiste em realizar pesquisas com possíveis clientes e buscar problemas, falhas e desafios para que nossa equipe possa solucioná-los.</t>
+  </si>
+  <si>
+    <t>DER001</t>
+  </si>
+  <si>
+    <t>O DER deverá ter uma tabela de usuário para fazer a captura de usuários.</t>
+  </si>
+  <si>
+    <t>Ao ser feito o cadastro pelo ADM, ele como administrador deverá cadastrar outros usuários.</t>
+  </si>
+  <si>
+    <t>O DER deverá ter uma tabela de perfil para para designar os niveis de permissões.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ao ser feito o cadastro do usuário o ADM deverá conceder a permissão que o usuário terá para acessar as dashboards. </t>
+  </si>
+  <si>
+    <t>O DER deverá ter uma tabela de cadastro-empresa para separar e atribuir a que empresa cada usuário pertence.</t>
+  </si>
+  <si>
+    <t>Ao ser cadastrado o ADM irá designar a qual empresa o usuário pertenci.</t>
+  </si>
+  <si>
+    <t>O DER deverá ter uma tabela de leitura para que seja feito o armazenamento e a transformação dos dados em interface gráfica.</t>
+  </si>
+  <si>
+    <t>Ao coletar dados das máquinas esses dados serão armazenados na tabela de leitura para serem apresentados nas dashboards.</t>
+  </si>
+  <si>
+    <t>O DER deverá ter uma tabela de unidade para o controle de qual unidade local, determinado totem pertenci.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ao ser feito o cadastro dos usuários, a unidade cadastrada será no determinado usuário será enviado para a tabela de unidade da qual ele pertenci.  </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Barlow"/>
+      </rPr>
+      <t>O DER deverá ter uma tabela de Totem</t>
+    </r>
     <r>
       <rPr>
         <b/>
@@ -266,7 +475,7 @@
         <color rgb="FF000000"/>
         <rFont val="Barlow"/>
       </rPr>
-      <t>Seção de serviços;</t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -274,289 +483,47 @@
         <color rgb="FF000000"/>
         <rFont val="Barlow"/>
       </rPr>
-      <t xml:space="preserve"> é um requisito importante para que caso os clientes tenha interesse sobre nossos serviços previamente possam ir até essa seção para conhecer e entrar em contato.</t>
+      <t>para identificação de cada máquina e que seja possível localiza-la.</t>
     </r>
   </si>
   <si>
-    <t>PROT004</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t>Seção de contato;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve"> é um requisito importante para que o cliente tenha acesso aos nossos serviços e possa entrar em contato; </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t>Seção de login;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve"> é um requisito importante para que o cliente tenha acesso ao nosso principal serviço, sendo ele as dashboards.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t>Seção de beneficios do negócio;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve"> é um requisito que apresenta ao usuário como nossos serviços funcionam e no que a equipe acredita.</t>
-    </r>
-  </si>
-  <si>
-    <t>PROT005</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve">Seção para ADM; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t>é um requisito importante pois é através desta seção que o usuário administrador pode fazer a criação de outros usuário analista.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve">Seção de dashboard para Analista; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t>é um requisito para que o analista responsavel da empresa possa ter acesso aos dados para tomada de decisão;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve">Seção de suporte; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t>é um requisito importante para que o usuário possa ter acesso a resolução de falhas e problemas nas dashboards.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve">Seção de cadastro; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t>é um requisito para que o ADM possa ser cadastrado.</t>
-    </r>
-  </si>
-  <si>
-    <t>EC001</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t>Pesquisa de campo;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve"> é um requisito importante para que a equipe possa identificar problemas, falhas e bugs nos sistemas operacionais dos totens de autoatendimento.</t>
-    </r>
-  </si>
-  <si>
-    <t>Desejável</t>
-  </si>
-  <si>
-    <t>DER001</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve">Tabela usuário; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t>é um requisito importante para que nosso banco de dados tenha as informações necessários sos usuários que que são cadastradas na nossa plataforma.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve">Tabela perfil; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t>é um requisito para que o sistema possa identificar o nível de permição de usuário.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t>Tabela cadastro-empresa;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve"> é um requisito para ter a separação de cada empresa e atribuir que usuários pertencem a ela.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t>Tabela de leitura;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve"> é um requisito para que seja feita o armazenamento dos dados e os mesmos sejam transformados em interface gráfica.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve">Tabela de unidade; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve"> é um requisito para o controle de que unidade local determinado totem pertenci.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t>Tabela de Totem;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Barlow"/>
-      </rPr>
-      <t xml:space="preserve"> é um requisito para identificação de cada máquina e que localiza-la.</t>
-    </r>
+    <t>Ao ser cadastrado o totem, o mesmo será ligado a unidade para que seja feita a sua localização.</t>
+  </si>
+  <si>
+    <t>US005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O site deverá apresentar dashboards com informações dos compartimentos do sistema de forma especifica.  </t>
+  </si>
+  <si>
+    <t>Ao usuário acessar a tela de dashboards o usuário terá acesso a informações especificas como cpu, memória, rede, disco etc...</t>
+  </si>
+  <si>
+    <t>US007</t>
+  </si>
+  <si>
+    <t>A tela de ADM deverá apresentar um icone com os usuários cadastrados para que o gerente tenha acesso a quem está analisando as telas de dashboard.</t>
+  </si>
+  <si>
+    <t>Ao ADM acessar sua tela como administrador ele terá acesso aos seus usuários cadastrados e a qual unidade ele pertenci.</t>
+  </si>
+  <si>
+    <t>US008</t>
+  </si>
+  <si>
+    <t>A tela de usuário deverá apresentar as telas de dashboard com os componentes especificos para serem analisados.</t>
+  </si>
+  <si>
+    <t>Ao usuário cadastrado acessar a tela de dashboard ele terá acesso aos gráficos para fazer a analise dos componentes.</t>
+  </si>
+  <si>
+    <t>US009</t>
+  </si>
+  <si>
+    <t>A tela de chamado de suporte deverá apresentar cartões com os problemas para que nossa equipe possa passar para o setor responsavél.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A equipe terá acesso a uma ferramenta para o gerenciamento de chamdos. </t>
   </si>
   <si>
     <t>Status</t>
@@ -670,26 +637,7 @@
     <t>EC</t>
   </si>
   <si>
-    <t>Product BackLog Qualified (PBQ) - Grupo 8</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">Menu de páginas; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>é um requisito para que o cliente e/ou usuário possa navegar pelas página principal e pelas outras paginas do site por completo.</t>
-    </r>
+    <t>Product BackLog Qualified (PBQ) - GRUPO 8</t>
   </si>
 </sst>
 </file>
@@ -699,7 +647,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -796,17 +744,6 @@
       <color rgb="FF000000"/>
       <name val="Barlow"/>
     </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-    </font>
   </fonts>
   <fills count="14">
     <fill>
@@ -1181,7 +1118,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1260,9 +1197,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1295,9 +1229,6 @@
     <xf numFmtId="0" fontId="12" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1359,13 +1290,26 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1383,26 +1327,26 @@
     </xf>
   </cellXfs>
   <cellStyles count="21">
-    <cellStyle name="Hiperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hiperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hiperlink Visitado" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hiperlink Visitado" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hiperlink Visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hiperlink Visitado" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="46">
@@ -2261,8 +2205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:I51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="23.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2281,618 +2225,716 @@
   <sheetData>
     <row r="1" spans="2:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" ht="89.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="62"/>
+      <c r="B2" s="62" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="64"/>
       <c r="I2"/>
     </row>
     <row r="3" spans="2:9" ht="9.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:9" s="25" customFormat="1" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="50" t="s">
+      <c r="C4" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="42" t="s">
+      <c r="E4" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="43" t="s">
+      <c r="F4" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="44" t="s">
+      <c r="G4" s="42" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:9" s="26" customFormat="1" ht="64.8" x14ac:dyDescent="0.25">
-      <c r="B5" s="45">
+    <row r="5" spans="2:9" s="26" customFormat="1" ht="69.599999999999994" x14ac:dyDescent="0.25">
+      <c r="B5" s="43">
         <v>1</v>
       </c>
-      <c r="C5" s="51" t="s">
+      <c r="C5" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="55" t="s">
+      <c r="E5" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="38" t="s">
+      <c r="F5" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="39"/>
-    </row>
-    <row r="6" spans="2:9" s="26" customFormat="1" ht="64.8" x14ac:dyDescent="0.25">
+      <c r="G5" s="57" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" s="26" customFormat="1" ht="86.4" x14ac:dyDescent="0.25">
       <c r="B6" s="27">
         <v>2</v>
       </c>
-      <c r="C6" s="52" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="30" t="s">
+      <c r="C6" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="57" t="s">
+      <c r="D6" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="38" t="s">
+      <c r="F6" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="31"/>
-    </row>
-    <row r="7" spans="2:9" s="26" customFormat="1" ht="36" x14ac:dyDescent="0.25">
-      <c r="B7" s="46">
+      <c r="G6" s="58" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" s="26" customFormat="1" ht="64.8" x14ac:dyDescent="0.25">
+      <c r="B7" s="44">
         <v>3</v>
       </c>
-      <c r="C7" s="51" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="30" t="s">
+      <c r="C7" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="58" t="s">
-        <v>84</v>
-      </c>
-      <c r="F7" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="31"/>
-    </row>
-    <row r="8" spans="2:9" s="26" customFormat="1" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="D7" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="61" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="58" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" s="26" customFormat="1" ht="86.4" x14ac:dyDescent="0.25">
       <c r="B8" s="27">
         <v>4</v>
       </c>
-      <c r="C8" s="51" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="30" t="s">
+      <c r="C8" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="55" t="s">
+      <c r="D8" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="31"/>
-    </row>
-    <row r="9" spans="2:9" s="26" customFormat="1" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="E8" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="58" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" s="26" customFormat="1" ht="52.2" x14ac:dyDescent="0.25">
       <c r="B9" s="27">
         <v>3</v>
       </c>
-      <c r="C9" s="51" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="30" t="s">
+      <c r="C9" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="55" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="31"/>
+      <c r="D9" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="58" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="10" spans="2:9" s="26" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="27">
         <v>4</v>
       </c>
-      <c r="C10" s="51" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="30" t="s">
+      <c r="C10" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="55" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="31"/>
-    </row>
-    <row r="11" spans="2:9" s="26" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="58" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" s="26" customFormat="1" ht="52.2" x14ac:dyDescent="0.25">
       <c r="B11" s="27">
         <v>5</v>
       </c>
-      <c r="C11" s="51" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="55" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="31"/>
-    </row>
-    <row r="12" spans="2:9" s="26" customFormat="1" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="C11" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="58" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" s="26" customFormat="1" ht="69.599999999999994" x14ac:dyDescent="0.25">
       <c r="B12" s="27">
         <v>6</v>
       </c>
-      <c r="C12" s="51" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="55" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="31"/>
-    </row>
-    <row r="13" spans="2:9" s="26" customFormat="1" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="C12" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="53" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="58" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" s="26" customFormat="1" ht="87" x14ac:dyDescent="0.25">
       <c r="B13" s="27">
         <v>7</v>
       </c>
-      <c r="C13" s="51" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="38" t="s">
+      <c r="C13" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="31"/>
-    </row>
-    <row r="14" spans="2:9" s="26" customFormat="1" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="G13" s="58" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" s="26" customFormat="1" ht="104.4" x14ac:dyDescent="0.25">
       <c r="B14" s="27">
         <v>8</v>
       </c>
-      <c r="C14" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="55" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" s="38" t="s">
+      <c r="C14" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="31"/>
-    </row>
-    <row r="15" spans="2:9" s="26" customFormat="1" ht="64.8" x14ac:dyDescent="0.25">
+      <c r="G14" s="58" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" s="26" customFormat="1" ht="69.599999999999994" x14ac:dyDescent="0.25">
       <c r="B15" s="27">
         <v>9</v>
       </c>
-      <c r="C15" s="51" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="31"/>
-    </row>
-    <row r="16" spans="2:9" s="26" customFormat="1" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="C15" s="49" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="58" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" s="26" customFormat="1" ht="52.2" x14ac:dyDescent="0.25">
       <c r="B16" s="27">
         <v>10</v>
       </c>
-      <c r="C16" s="52" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="55" t="s">
-        <v>28</v>
-      </c>
-      <c r="F16" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="31"/>
-    </row>
-    <row r="17" spans="2:7" s="26" customFormat="1" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="C16" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="58" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" s="26" customFormat="1" ht="104.4" x14ac:dyDescent="0.25">
       <c r="B17" s="27">
         <v>11</v>
       </c>
-      <c r="C17" s="51" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="F17" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="31"/>
-    </row>
-    <row r="18" spans="2:7" s="26" customFormat="1" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="C17" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="58" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" s="26" customFormat="1" ht="52.2" x14ac:dyDescent="0.25">
       <c r="B18" s="27">
         <v>12</v>
       </c>
-      <c r="C18" s="51" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="30" t="s">
+      <c r="C18" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="55" t="s">
-        <v>30</v>
-      </c>
-      <c r="F18" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="G18" s="31"/>
-    </row>
-    <row r="19" spans="2:7" s="26" customFormat="1" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="D18" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="58" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" s="26" customFormat="1" ht="87" x14ac:dyDescent="0.25">
       <c r="B19" s="27">
         <v>13</v>
       </c>
-      <c r="C19" s="51" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="E19" s="55" t="s">
-        <v>32</v>
-      </c>
-      <c r="F19" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="G19" s="31"/>
-    </row>
-    <row r="20" spans="2:7" s="26" customFormat="1" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="C19" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="53" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="58" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" s="26" customFormat="1" ht="87" x14ac:dyDescent="0.25">
       <c r="B20" s="27">
         <v>14</v>
       </c>
-      <c r="C20" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20" s="55" t="s">
-        <v>33</v>
-      </c>
-      <c r="F20" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="G20" s="31"/>
-    </row>
-    <row r="21" spans="2:7" s="26" customFormat="1" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="C20" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="53" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="58" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" s="26" customFormat="1" ht="69.599999999999994" x14ac:dyDescent="0.25">
       <c r="B21" s="27">
         <v>15</v>
       </c>
-      <c r="C21" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" s="55" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="G21" s="31"/>
-    </row>
-    <row r="22" spans="2:7" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="58" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" s="26" customFormat="1" ht="69.599999999999994" x14ac:dyDescent="0.25">
       <c r="B22" s="27">
         <v>16</v>
       </c>
-      <c r="C22" s="52" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="56" t="s">
-        <v>35</v>
-      </c>
-      <c r="F22" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="G22" s="31"/>
-    </row>
-    <row r="23" spans="2:7" s="26" customFormat="1" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="C22" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="58" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" s="26" customFormat="1" ht="69.599999999999994" x14ac:dyDescent="0.25">
       <c r="B23" s="27">
         <v>17</v>
       </c>
-      <c r="C23" s="52" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="E23" s="55" t="s">
-        <v>37</v>
-      </c>
-      <c r="F23" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="G23" s="31"/>
-    </row>
-    <row r="24" spans="2:7" s="26" customFormat="1" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="C23" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="53" t="s">
+        <v>55</v>
+      </c>
+      <c r="F23" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" s="58" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" s="26" customFormat="1" ht="52.2" x14ac:dyDescent="0.25">
       <c r="B24" s="27">
         <v>18</v>
       </c>
-      <c r="C24" s="52" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" s="55" t="s">
-        <v>40</v>
-      </c>
-      <c r="F24" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="G24" s="31"/>
-    </row>
-    <row r="25" spans="2:7" s="26" customFormat="1" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="C24" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="53" t="s">
+        <v>59</v>
+      </c>
+      <c r="F24" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" s="58" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" s="26" customFormat="1" ht="52.2" x14ac:dyDescent="0.25">
       <c r="B25" s="27">
         <v>19</v>
       </c>
-      <c r="C25" s="52" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="55" t="s">
-        <v>41</v>
-      </c>
-      <c r="F25" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="G25" s="31"/>
-    </row>
-    <row r="26" spans="2:7" s="26" customFormat="1" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="C25" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="53" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" s="58" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" s="26" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.25">
       <c r="B26" s="27">
         <v>20</v>
       </c>
-      <c r="C26" s="52" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="E26" s="59" t="s">
-        <v>42</v>
-      </c>
-      <c r="F26" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="G26" s="31"/>
-    </row>
-    <row r="27" spans="2:7" s="26" customFormat="1" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="C26" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="56" t="s">
+        <v>63</v>
+      </c>
+      <c r="F26" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" s="58" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" s="26" customFormat="1" ht="69.599999999999994" x14ac:dyDescent="0.25">
       <c r="B27" s="27">
         <v>21</v>
       </c>
-      <c r="C27" s="52" t="s">
-        <v>39</v>
-      </c>
-      <c r="D27" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="E27" s="55" t="s">
-        <v>43</v>
-      </c>
-      <c r="F27" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="G27" s="31"/>
-    </row>
-    <row r="28" spans="2:7" s="26" customFormat="1" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="C27" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="F27" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="G27" s="58" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" s="26" customFormat="1" ht="69.599999999999994" x14ac:dyDescent="0.25">
       <c r="B28" s="27">
         <v>22</v>
       </c>
-      <c r="C28" s="52" t="s">
-        <v>39</v>
-      </c>
-      <c r="D28" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="E28" s="55" t="s">
-        <v>44</v>
-      </c>
-      <c r="F28" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="G28" s="31"/>
-    </row>
-    <row r="29" spans="2:7" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="F28" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="G28" s="58" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" s="26" customFormat="1" ht="52.2" x14ac:dyDescent="0.25">
       <c r="B29" s="27">
         <v>23</v>
       </c>
-      <c r="C29" s="52" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="E29" s="55" t="s">
-        <v>45</v>
-      </c>
-      <c r="F29" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="G29" s="31"/>
-    </row>
-    <row r="30" spans="2:7" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="27"/>
-      <c r="C30" s="52"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="31"/>
-    </row>
-    <row r="31" spans="2:7" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="27"/>
-      <c r="C31" s="52"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="31"/>
-    </row>
-    <row r="32" spans="2:7" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="27"/>
-      <c r="C32" s="52"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="31"/>
-    </row>
-    <row r="33" spans="2:7" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="27"/>
-      <c r="C33" s="52"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="31"/>
+      <c r="C29" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="G29" s="58" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" s="26" customFormat="1" ht="69.599999999999994" x14ac:dyDescent="0.25">
+      <c r="B30" s="27">
+        <v>24</v>
+      </c>
+      <c r="C30" s="50" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E30" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="F30" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="G30" s="58" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" s="26" customFormat="1" ht="69.599999999999994" x14ac:dyDescent="0.25">
+      <c r="B31" s="27">
+        <v>25</v>
+      </c>
+      <c r="C31" s="50" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="F31" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" s="58" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" s="26" customFormat="1" ht="52.2" x14ac:dyDescent="0.25">
+      <c r="B32" s="27">
+        <v>26</v>
+      </c>
+      <c r="C32" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" s="59" t="s">
+        <v>78</v>
+      </c>
+      <c r="F32" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" s="58" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" s="26" customFormat="1" ht="34.799999999999997" x14ac:dyDescent="0.25">
+      <c r="B33" s="27">
+        <v>27</v>
+      </c>
+      <c r="C33" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="D33" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" s="59" t="s">
+        <v>81</v>
+      </c>
+      <c r="F33" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" s="58" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="34" spans="2:7" s="26" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="27"/>
-      <c r="C34" s="52"/>
-      <c r="D34" s="30"/>
+      <c r="C34" s="50"/>
+      <c r="D34" s="29"/>
       <c r="E34" s="27"/>
-      <c r="F34" s="28"/>
-      <c r="G34" s="31"/>
+      <c r="F34" s="60"/>
+      <c r="G34" s="30"/>
     </row>
     <row r="35" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="47"/>
-      <c r="C35" s="53"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="33"/>
+      <c r="B35" s="45"/>
+      <c r="C35" s="51"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="32"/>
     </row>
     <row r="36" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="47"/>
-      <c r="C36" s="53"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="29"/>
-      <c r="G36" s="33"/>
+      <c r="B36" s="45"/>
+      <c r="C36" s="51"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="32"/>
     </row>
     <row r="37" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="47"/>
-      <c r="C37" s="53"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="33"/>
+      <c r="B37" s="45"/>
+      <c r="C37" s="51"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="32"/>
     </row>
     <row r="38" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="47"/>
-      <c r="C38" s="53"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="33"/>
+      <c r="B38" s="45"/>
+      <c r="C38" s="51"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="32"/>
     </row>
     <row r="39" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="47"/>
-      <c r="C39" s="53"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="29"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="33"/>
+      <c r="B39" s="45"/>
+      <c r="C39" s="51"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="32"/>
     </row>
     <row r="40" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="48"/>
-      <c r="C40" s="54"/>
-      <c r="D40" s="34"/>
-      <c r="E40" s="35"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="36"/>
+      <c r="B40" s="46"/>
+      <c r="C40" s="52"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="34"/>
+      <c r="G40" s="35"/>
     </row>
     <row r="41" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="49"/>
-      <c r="C41" s="49"/>
+      <c r="B41" s="47"/>
+      <c r="C41" s="47"/>
       <c r="F41" s="16"/>
     </row>
     <row r="42" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="49"/>
-      <c r="C42" s="49"/>
+      <c r="B42" s="47"/>
+      <c r="C42" s="47"/>
       <c r="F42" s="16"/>
     </row>
     <row r="43" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="49"/>
-      <c r="C43" s="49"/>
+      <c r="B43" s="47"/>
+      <c r="C43" s="47"/>
       <c r="F43" s="16"/>
     </row>
     <row r="44" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="49"/>
-      <c r="C44" s="49"/>
+      <c r="B44" s="47"/>
+      <c r="C44" s="47"/>
       <c r="F44" s="16"/>
     </row>
     <row r="45" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="49"/>
-      <c r="C45" s="49"/>
+      <c r="B45" s="47"/>
+      <c r="C45" s="47"/>
       <c r="F45" s="16"/>
     </row>
     <row r="46" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="49"/>
-      <c r="C46" s="49"/>
+      <c r="B46" s="47"/>
+      <c r="C46" s="47"/>
       <c r="F46" s="16"/>
     </row>
     <row r="47" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="49"/>
-      <c r="C47" s="49"/>
+      <c r="B47" s="47"/>
+      <c r="C47" s="47"/>
       <c r="F47" s="16"/>
     </row>
     <row r="48" spans="2:7" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="49"/>
-      <c r="C48" s="49"/>
+      <c r="B48" s="47"/>
+      <c r="C48" s="47"/>
       <c r="F48" s="16"/>
     </row>
     <row r="49" spans="2:6" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="49"/>
-      <c r="C49" s="49"/>
+      <c r="B49" s="47"/>
+      <c r="C49" s="47"/>
       <c r="F49" s="16"/>
     </row>
     <row r="50" spans="2:6" s="15" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -3076,13 +3118,13 @@
           <x14:formula1>
             <xm:f>Dados!$A$2:$A$14</xm:f>
           </x14:formula1>
-          <xm:sqref>F30:F34</xm:sqref>
+          <xm:sqref>F34</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A02F1AAD-E838-4EC2-BAE2-D30AC13FC4E6}">
           <x14:formula1>
             <xm:f>Dados!$E$2:$E$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F5:F29</xm:sqref>
+          <xm:sqref>F5:F33</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000001000000}">
           <x14:formula1>
@@ -3103,8 +3145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
@@ -3119,10 +3161,10 @@
     <row r="1" spans="1:11" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22"/>
       <c r="B1" s="23" t="s">
-        <v>46</v>
+        <v>83</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>4</v>
@@ -3131,30 +3173,30 @@
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" s="18" t="s">
-        <v>48</v>
+        <v>85</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>49</v>
+        <v>86</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H2" s="64" t="s">
-        <v>50</v>
-      </c>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
+        <v>56</v>
+      </c>
+      <c r="H2" s="66" t="s">
+        <v>87</v>
+      </c>
+      <c r="I2" s="66"/>
+      <c r="J2" s="66"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3" s="18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="8"/>
@@ -3163,13 +3205,13 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
       <c r="B4" s="18" t="s">
-        <v>52</v>
+        <v>89</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="H4" s="9"/>
       <c r="I4" s="10"/>
@@ -3178,22 +3220,22 @@
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
       <c r="B5" s="18" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="H5" s="63"/>
-      <c r="I5" s="63"/>
-      <c r="J5" s="63"/>
+        <v>91</v>
+      </c>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="65"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="18"/>
       <c r="B6" s="18" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>55</v>
+        <v>92</v>
       </c>
       <c r="K6" s="13"/>
     </row>
@@ -3201,28 +3243,28 @@
       <c r="A7" s="18"/>
       <c r="B7" s="18"/>
       <c r="C7" s="19" t="s">
-        <v>56</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
       <c r="B8" s="18"/>
       <c r="C8" s="19" t="s">
-        <v>57</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
       <c r="B9" s="18"/>
       <c r="C9" s="19" t="s">
-        <v>58</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10" s="18"/>
       <c r="C10" s="19" t="s">
-        <v>59</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -3247,98 +3289,98 @@
     </row>
     <row r="16" spans="1:11" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
-        <v>60</v>
+        <v>97</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>61</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
-        <v>62</v>
+        <v>99</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>62</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
-        <v>63</v>
+        <v>100</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>64</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
-        <v>65</v>
+        <v>102</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>68</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
-        <v>69</v>
+        <v>106</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>70</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
-        <v>71</v>
+        <v>108</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>72</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
-        <v>73</v>
+        <v>110</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>74</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A24" s="21" t="s">
-        <v>75</v>
+        <v>112</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>76</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A25" s="21" t="s">
-        <v>77</v>
+        <v>114</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>78</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
-        <v>79</v>
+        <v>116</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>80</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="23.4" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
-        <v>81</v>
+        <v>118</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>82</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -3357,12 +3399,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101007ACFDD1B2CAD7546B60E55C07A86393C" ma:contentTypeVersion="2" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="181a36d502e7a0b748a7cd3f44c84256">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="93df9749-2e2e-4b03-97b6-02f28a4f49b8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="72d2526e4fdcc8fa6c9a35e442f2e6a0" ns2:_="">
     <xsd:import namespace="93df9749-2e2e-4b03-97b6-02f28a4f49b8"/>
@@ -3494,7 +3530,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -3503,16 +3539,13 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FCF2672-EA77-4AF1-BE56-97AA2FBEFF47}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10A50834-C7D8-4E98-BE58-A043B5E9C339}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3530,10 +3563,26 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92EF175B-F78D-4CB0-A5EB-3F12E9CE216A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FCF2672-EA77-4AF1-BE56-97AA2FBEFF47}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="93df9749-2e2e-4b03-97b6-02f28a4f49b8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>